<commit_message>
Prep labels complete without indivisible pack error
</commit_message>
<xml_diff>
--- a/Python_ASN_Bot/Label_Prep_Status.xlsx
+++ b/Python_ASN_Bot/Label_Prep_Status.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,146 +463,146 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>35247161991</t>
+          <t>35247173151</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ABE4</t>
+          <t>CHA2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247161991&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173151&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>35247170011</t>
+          <t>35247212391</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ACY2</t>
+          <t>CMH2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247170011&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212391&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>35247212431</t>
+          <t>35247210891</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BNA2</t>
+          <t>MCI3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212431&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210891&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>35247161981</t>
+          <t>35247192681</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BNA6</t>
+          <t>MCO2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247161981&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247192681&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>35247210841</t>
+          <t>35247210901</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BOS7</t>
+          <t>MDW6</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210841&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210901&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Complete</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>35247173151</t>
+          <t>35247173191</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHA2</t>
+          <t>MDW9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173151&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173191&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -613,46 +613,46 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>35247210851</t>
+          <t>35247173221</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CLT3</t>
+          <t>OAK3</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210851&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173221&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Already Completed</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>35247212391</t>
+          <t>35247210911</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CMH2</t>
+          <t>PBI3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212391&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210911&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -663,17 +663,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>35247212421</t>
+          <t>35247212481</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DFW6</t>
+          <t>PHL6</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212421&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212481&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -688,46 +688,46 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>35247212441</t>
+          <t>35247173201</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>IND2</t>
+          <t>PHX7</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212441&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173201&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>35247210891</t>
+          <t>35247175821</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MCI3</t>
+          <t>PPO4</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210891&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247175821&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -738,21 +738,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>35247192681</t>
+          <t>35247212521</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MCO2</t>
+          <t>RDU4</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247192681&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212521&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -763,21 +763,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>35247210901</t>
+          <t>35247158701</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MDW6</t>
+          <t>RYY2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210901&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247158701&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -788,17 +788,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>35247173191</t>
+          <t>35247192711</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MDW9</t>
+          <t>SAT1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173191&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247192711&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -813,21 +813,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>35247173221</t>
+          <t>35247212531</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OAK3</t>
+          <t>SBD2</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173221&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212531&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -838,42 +838,42 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>35247210911</t>
+          <t>35247212451</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PBI3</t>
+          <t>SNA4</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247210911&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212451&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>35247212481</t>
+          <t>35247173251</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PHL6</t>
+          <t>STL6</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212481&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173251&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -888,21 +888,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>35247173201</t>
+          <t>35247175831</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>PHX7</t>
+          <t>TEB3</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173201&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247175831&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -913,21 +913,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>35247175821</t>
+          <t>35247173261</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PPO4</t>
+          <t>TPA2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247175821&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173261&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -938,21 +938,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>35247212521</t>
+          <t>35247212551</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RDU4</t>
+          <t>TPA3</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212521&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212551&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -963,248 +963,23 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>35247158701</t>
+          <t>35247173241</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RYY2</t>
+          <t>TTN2</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247158701&amp;isLegacy=false</t>
+          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173241&amp;isLegacy=false</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>35247192711</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>SAT1</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247192711&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>35247212531</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>SBD2</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212531&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>4</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>35247212451</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>SNA4</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212451&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>3</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>35247173251</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>STL6</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173251&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>35247175831</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>TEB3</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247175831&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>35247173261</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>TPA2</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173261&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>2</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>35247212551</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>TPA3</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247212551&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>35247173241</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>TTN2</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173241&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D30" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>35247173291</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>WBW2</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>https://vendorcentral.amazon.com/kt/vendor/members/afi-shipment-mgr/labelmapping?arn=35247173291&amp;isLegacy=false</t>
-        </is>
-      </c>
-      <c r="D31" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" t="inlineStr">
         <is>
           <t>Complete</t>
         </is>

</xml_diff>